<commit_message>
Simplified code, fixed template
</commit_message>
<xml_diff>
--- a/src/jvmMain/resources/TeamExpenseBreakdownTemplate.xlsx
+++ b/src/jvmMain/resources/TeamExpenseBreakdownTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Documents\Spring 2023\CS-481\s23-totalled\src\jvmMain\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DFC079-DD73-4CCF-9E8C-E10205D52289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC96E5-D99F-430E-9C6B-BEC23B21D504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,17 +125,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -193,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -226,14 +215,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,7 +440,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A6" sqref="A6:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -477,16 +458,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -558,7 +539,7 @@
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="13"/>
@@ -686,25 +667,25 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
@@ -722,14 +703,14 @@
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>

</xml_diff>

<commit_message>
[#129] clean up lineitemwriter.kt (#144)
</commit_message>
<xml_diff>
--- a/src/jvmMain/resources/TeamExpenseBreakdownTemplate.xlsx
+++ b/src/jvmMain/resources/TeamExpenseBreakdownTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12088\Documents\Spring 2023\CS-481\s23-totalled\src\jvmMain\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DFC079-DD73-4CCF-9E8C-E10205D52289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC96E5-D99F-430E-9C6B-BEC23B21D504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,17 +125,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -193,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -226,14 +215,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,7 +440,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A6" sqref="A6:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -477,16 +458,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -558,7 +539,7 @@
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="13"/>
@@ -686,25 +667,25 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
@@ -722,14 +703,14 @@
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>

</xml_diff>